<commit_message>
Excel file was update
</commit_message>
<xml_diff>
--- a/Role permissions.xlsx
+++ b/Role permissions.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20325"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{24976A5D-58A2-4D84-AE74-FAFE841C493C}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{221B9E96-B9BB-41BC-BF1F-B71B23B75A78}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-105" yWindow="-105" windowWidth="23250" windowHeight="12570" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="56">
   <si>
     <t>/compound/add [GET]</t>
   </si>
@@ -182,6 +182,12 @@
   </si>
   <si>
     <t>QA</t>
+  </si>
+  <si>
+    <t>HR("HR Manager")</t>
+  </si>
+  <si>
+    <t>ACC("Accountant")</t>
   </si>
 </sst>
 </file>
@@ -569,19 +575,22 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B2:J46"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H28" sqref="H28"/>
+    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="42" customWidth="1"/>
-    <col min="3" max="3" width="17.6640625" customWidth="1"/>
-    <col min="4" max="4" width="15.88671875" customWidth="1"/>
-    <col min="5" max="7" width="13.6640625" customWidth="1"/>
+    <col min="2" max="2" width="44.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.7109375" customWidth="1"/>
+    <col min="6" max="6" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="8.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:10" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="2" spans="2:10" ht="45" x14ac:dyDescent="0.25">
       <c r="B2" s="2"/>
       <c r="C2" s="4" t="s">
         <v>44</v>
@@ -598,11 +607,15 @@
       <c r="G2" s="4" t="s">
         <v>47</v>
       </c>
-      <c r="H2" s="1"/>
-      <c r="I2" s="1"/>
+      <c r="H2" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="I2" s="1" t="s">
+        <v>55</v>
+      </c>
       <c r="J2" s="1"/>
     </row>
-    <row r="3" spans="2:10" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B3" s="2" t="s">
         <v>0</v>
       </c>
@@ -616,7 +629,7 @@
       </c>
       <c r="G3" s="5"/>
     </row>
-    <row r="4" spans="2:10" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B4" s="2" t="s">
         <v>1</v>
       </c>
@@ -626,7 +639,7 @@
       <c r="F4" s="5"/>
       <c r="G4" s="5"/>
     </row>
-    <row r="5" spans="2:10" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B5" s="2" t="s">
         <v>2</v>
       </c>
@@ -640,7 +653,7 @@
       </c>
       <c r="G5" s="5"/>
     </row>
-    <row r="6" spans="2:10" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="6" spans="2:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B6" s="2" t="s">
         <v>3</v>
       </c>
@@ -658,7 +671,7 @@
       </c>
       <c r="G6" s="5"/>
     </row>
-    <row r="7" spans="2:10" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="7" spans="2:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B7" s="2" t="s">
         <v>4</v>
       </c>
@@ -672,7 +685,7 @@
       </c>
       <c r="G7" s="5"/>
     </row>
-    <row r="8" spans="2:10" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="8" spans="2:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B8" s="2" t="s">
         <v>5</v>
       </c>
@@ -684,7 +697,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="9" spans="2:10" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="9" spans="2:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B9" s="2" t="s">
         <v>6</v>
       </c>
@@ -694,7 +707,7 @@
       <c r="F9" s="5"/>
       <c r="G9" s="5"/>
     </row>
-    <row r="10" spans="2:10" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="10" spans="2:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B10" s="2" t="s">
         <v>7</v>
       </c>
@@ -707,7 +720,7 @@
       </c>
       <c r="J10" s="3"/>
     </row>
-    <row r="11" spans="2:10" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="11" spans="2:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B11" s="2" t="s">
         <v>8</v>
       </c>
@@ -719,7 +732,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="12" spans="2:10" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="12" spans="2:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B12" s="2" t="s">
         <v>9</v>
       </c>
@@ -733,7 +746,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="13" spans="2:10" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="13" spans="2:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B13" s="2" t="s">
         <v>10</v>
       </c>
@@ -743,7 +756,7 @@
       <c r="F13" s="5"/>
       <c r="G13" s="5"/>
     </row>
-    <row r="14" spans="2:10" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="14" spans="2:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B14" s="2" t="s">
         <v>11</v>
       </c>
@@ -757,7 +770,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="15" spans="2:10" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="15" spans="2:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B15" s="2" t="s">
         <v>12</v>
       </c>
@@ -769,7 +782,7 @@
       <c r="F15" s="5"/>
       <c r="G15" s="5"/>
     </row>
-    <row r="16" spans="2:10" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="16" spans="2:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B16" s="2" t="s">
         <v>13</v>
       </c>
@@ -781,7 +794,7 @@
       <c r="F16" s="5"/>
       <c r="G16" s="5"/>
     </row>
-    <row r="17" spans="2:7" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B17" s="2" t="s">
         <v>14</v>
       </c>
@@ -793,7 +806,7 @@
       <c r="F17" s="5"/>
       <c r="G17" s="5"/>
     </row>
-    <row r="18" spans="2:7" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="18" spans="2:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B18" s="2" t="s">
         <v>15</v>
       </c>
@@ -803,7 +816,7 @@
       <c r="F18" s="5"/>
       <c r="G18" s="5"/>
     </row>
-    <row r="19" spans="2:7" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="19" spans="2:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B19" s="2" t="s">
         <v>16</v>
       </c>
@@ -823,7 +836,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="20" spans="2:7" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="20" spans="2:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B20" s="2" t="s">
         <v>17</v>
       </c>
@@ -843,7 +856,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="21" spans="2:7" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="21" spans="2:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B21" s="2" t="s">
         <v>18</v>
       </c>
@@ -863,7 +876,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="22" spans="2:7" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="22" spans="2:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B22" s="2" t="s">
         <v>19</v>
       </c>
@@ -877,7 +890,7 @@
       </c>
       <c r="G22" s="5"/>
     </row>
-    <row r="23" spans="2:7" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="23" spans="2:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B23" s="2" t="s">
         <v>20</v>
       </c>
@@ -891,7 +904,7 @@
       </c>
       <c r="G23" s="5"/>
     </row>
-    <row r="24" spans="2:7" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="24" spans="2:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B24" s="2" t="s">
         <v>21</v>
       </c>
@@ -905,7 +918,7 @@
       </c>
       <c r="G24" s="5"/>
     </row>
-    <row r="25" spans="2:7" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="25" spans="2:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B25" s="2" t="s">
         <v>22</v>
       </c>
@@ -923,7 +936,7 @@
       </c>
       <c r="G25" s="5"/>
     </row>
-    <row r="26" spans="2:7" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="26" spans="2:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B26" s="2" t="s">
         <v>23</v>
       </c>
@@ -935,7 +948,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="27" spans="2:7" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="27" spans="2:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B27" s="2" t="s">
         <v>24</v>
       </c>
@@ -945,7 +958,7 @@
       <c r="F27" s="5"/>
       <c r="G27" s="5"/>
     </row>
-    <row r="28" spans="2:7" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="28" spans="2:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B28" s="2" t="s">
         <v>25</v>
       </c>
@@ -957,7 +970,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="29" spans="2:7" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="29" spans="2:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B29" s="2" t="s">
         <v>26</v>
       </c>
@@ -969,7 +982,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="30" spans="2:7" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="30" spans="2:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B30" s="2" t="s">
         <v>27</v>
       </c>
@@ -981,7 +994,7 @@
       <c r="F30" s="5"/>
       <c r="G30" s="5"/>
     </row>
-    <row r="31" spans="2:7" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="31" spans="2:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B31" s="2" t="s">
         <v>28</v>
       </c>
@@ -993,7 +1006,7 @@
       <c r="F31" s="5"/>
       <c r="G31" s="5"/>
     </row>
-    <row r="32" spans="2:7" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="32" spans="2:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B32" s="2" t="s">
         <v>29</v>
       </c>
@@ -1005,7 +1018,7 @@
       <c r="F32" s="5"/>
       <c r="G32" s="5"/>
     </row>
-    <row r="33" spans="2:7" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="33" spans="2:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B33" s="2" t="s">
         <v>30</v>
       </c>
@@ -1017,7 +1030,7 @@
       <c r="F33" s="5"/>
       <c r="G33" s="5"/>
     </row>
-    <row r="34" spans="2:7" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="34" spans="2:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B34" s="2" t="s">
         <v>31</v>
       </c>
@@ -1029,7 +1042,7 @@
       <c r="F34" s="5"/>
       <c r="G34" s="5"/>
     </row>
-    <row r="35" spans="2:7" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="35" spans="2:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B35" s="2" t="s">
         <v>32</v>
       </c>
@@ -1043,7 +1056,7 @@
       </c>
       <c r="G35" s="5"/>
     </row>
-    <row r="36" spans="2:7" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="36" spans="2:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B36" s="2" t="s">
         <v>33</v>
       </c>
@@ -1057,7 +1070,7 @@
       </c>
       <c r="G36" s="5"/>
     </row>
-    <row r="37" spans="2:7" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="37" spans="2:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B37" s="2" t="s">
         <v>34</v>
       </c>
@@ -1071,7 +1084,7 @@
       </c>
       <c r="G37" s="5"/>
     </row>
-    <row r="38" spans="2:7" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="38" spans="2:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B38" s="2" t="s">
         <v>35</v>
       </c>
@@ -1085,7 +1098,7 @@
       </c>
       <c r="G38" s="5"/>
     </row>
-    <row r="39" spans="2:7" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="39" spans="2:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B39" s="2" t="s">
         <v>36</v>
       </c>
@@ -1097,7 +1110,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="40" spans="2:7" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="40" spans="2:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B40" s="2" t="s">
         <v>37</v>
       </c>
@@ -1107,7 +1120,7 @@
       <c r="F40" s="5"/>
       <c r="G40" s="5"/>
     </row>
-    <row r="41" spans="2:7" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="41" spans="2:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B41" s="2" t="s">
         <v>38</v>
       </c>
@@ -1119,7 +1132,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="42" spans="2:7" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="42" spans="2:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B42" s="2" t="s">
         <v>39</v>
       </c>
@@ -1131,7 +1144,7 @@
       <c r="F42" s="5"/>
       <c r="G42" s="5"/>
     </row>
-    <row r="43" spans="2:7" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="43" spans="2:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B43" s="2" t="s">
         <v>40</v>
       </c>
@@ -1143,7 +1156,7 @@
       <c r="F43" s="5"/>
       <c r="G43" s="5"/>
     </row>
-    <row r="44" spans="2:7" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="44" spans="2:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B44" s="2" t="s">
         <v>41</v>
       </c>
@@ -1153,7 +1166,7 @@
       <c r="F44" s="5"/>
       <c r="G44" s="5"/>
     </row>
-    <row r="45" spans="2:7" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="45" spans="2:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B45" s="2" t="s">
         <v>42</v>
       </c>
@@ -1165,7 +1178,7 @@
       <c r="F45" s="5"/>
       <c r="G45" s="5"/>
     </row>
-    <row r="46" spans="2:7" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="46" spans="2:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B46" s="2" t="s">
         <v>43</v>
       </c>

</xml_diff>

<commit_message>
Email Service partially completed
</commit_message>
<xml_diff>
--- a/Role permissions.xlsx
+++ b/Role permissions.xlsx
@@ -3,14 +3,15 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21328"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5417616F-3BA1-4245-85B0-0E0CA08699E6}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DB1A3E51-F55C-4250-81D2-AC7AB9A49FC5}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="181029"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -770,8 +771,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B2:Q46"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="M26" sqref="M26"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="K15" sqref="K15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>

</xml_diff>

<commit_message>
Role permission added in navBar.html
</commit_message>
<xml_diff>
--- a/Role permissions.xlsx
+++ b/Role permissions.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21328"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0FC1AF91-3539-41FF-BE1A-A7069702B19C}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6609DC37-178D-471C-98B1-B728D0B15541}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="220" uniqueCount="100">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="916" uniqueCount="101">
   <si>
     <t>/compound/add [GET]</t>
   </si>
@@ -364,6 +364,9 @@
   </si>
   <si>
     <t>after payment</t>
+  </si>
+  <si>
+    <t>ADMIN</t>
   </si>
 </sst>
 </file>
@@ -409,7 +412,7 @@
       <family val="3"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -431,6 +434,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -463,7 +472,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -488,6 +497,12 @@
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -777,10 +792,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B2:Q46"/>
+  <dimension ref="B2:R46"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C5" workbookViewId="0">
-      <selection activeCell="M25" sqref="M25"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J43" sqref="J43:J46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -792,13 +807,13 @@
     <col min="6" max="6" width="11.88671875" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="13.33203125" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="8.6640625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="34.44140625" customWidth="1"/>
-    <col min="14" max="14" width="24.6640625" customWidth="1"/>
-    <col min="15" max="15" width="6.21875" customWidth="1"/>
-    <col min="16" max="16" width="25.5546875" customWidth="1"/>
+    <col min="14" max="14" width="34.44140625" customWidth="1"/>
+    <col min="15" max="15" width="24.6640625" customWidth="1"/>
+    <col min="16" max="16" width="6.21875" customWidth="1"/>
+    <col min="17" max="17" width="25.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:17" ht="43.2">
+    <row r="2" spans="2:18" ht="43.2">
       <c r="B2" s="2"/>
       <c r="C2" s="4" t="s">
         <v>44</v>
@@ -815,30 +830,33 @@
       <c r="G2" s="4" t="s">
         <v>47</v>
       </c>
-      <c r="H2" s="1" t="s">
+      <c r="H2" s="10" t="s">
         <v>54</v>
       </c>
-      <c r="I2" s="1" t="s">
+      <c r="I2" s="10" t="s">
         <v>55</v>
       </c>
-      <c r="J2" s="1"/>
-      <c r="M2" s="7" t="s">
+      <c r="J2" s="10" t="s">
+        <v>100</v>
+      </c>
+      <c r="K2" s="1"/>
+      <c r="N2" s="7" t="s">
         <v>79</v>
       </c>
-      <c r="N2" t="s">
+      <c r="O2" t="s">
         <v>59</v>
       </c>
-      <c r="O2" s="8" t="s">
+      <c r="P2" s="8" t="s">
         <v>80</v>
       </c>
-      <c r="P2" t="s">
+      <c r="Q2" t="s">
         <v>60</v>
       </c>
-      <c r="Q2" s="7" t="s">
+      <c r="R2" s="7" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="3" spans="2:17" ht="15.6">
+    <row r="3" spans="2:18" ht="15.6">
       <c r="B3" s="2" t="s">
         <v>0</v>
       </c>
@@ -851,23 +869,26 @@
         <v>50</v>
       </c>
       <c r="G3" s="5"/>
-      <c r="M3" s="7" t="s">
+      <c r="H3" s="12"/>
+      <c r="I3" s="12"/>
+      <c r="J3" s="13"/>
+      <c r="N3" s="7" t="s">
         <v>79</v>
       </c>
-      <c r="N3" t="s">
+      <c r="O3" t="s">
         <v>61</v>
       </c>
-      <c r="O3" s="8" t="s">
+      <c r="P3" s="8" t="s">
         <v>80</v>
       </c>
-      <c r="P3" t="s">
+      <c r="Q3" t="s">
         <v>62</v>
       </c>
-      <c r="Q3" s="7" t="s">
+      <c r="R3" s="7" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="4" spans="2:17" ht="15.6">
+    <row r="4" spans="2:18" ht="15.6">
       <c r="B4" s="2" t="s">
         <v>1</v>
       </c>
@@ -876,23 +897,26 @@
       <c r="E4" s="5"/>
       <c r="F4" s="5"/>
       <c r="G4" s="5"/>
-      <c r="M4" s="7" t="s">
+      <c r="H4" s="12"/>
+      <c r="I4" s="12"/>
+      <c r="J4" s="13"/>
+      <c r="N4" s="7" t="s">
         <v>79</v>
       </c>
-      <c r="N4" t="s">
+      <c r="O4" t="s">
         <v>63</v>
       </c>
-      <c r="O4" s="8" t="s">
+      <c r="P4" s="8" t="s">
         <v>80</v>
       </c>
-      <c r="P4" t="s">
+      <c r="Q4" t="s">
         <v>78</v>
       </c>
-      <c r="Q4" s="7" t="s">
+      <c r="R4" s="7" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="5" spans="2:17" ht="15.6">
+    <row r="5" spans="2:18" ht="15.6">
       <c r="B5" s="2" t="s">
         <v>2</v>
       </c>
@@ -905,23 +929,26 @@
         <v>50</v>
       </c>
       <c r="G5" s="5"/>
-      <c r="M5" s="7" t="s">
+      <c r="H5" s="12"/>
+      <c r="I5" s="12"/>
+      <c r="J5" s="13"/>
+      <c r="N5" s="7" t="s">
         <v>79</v>
       </c>
-      <c r="N5" t="s">
+      <c r="O5" t="s">
         <v>64</v>
       </c>
-      <c r="O5" s="8" t="s">
+      <c r="P5" s="8" t="s">
         <v>80</v>
       </c>
-      <c r="P5" t="s">
+      <c r="Q5" t="s">
         <v>66</v>
       </c>
-      <c r="Q5" s="7" t="s">
+      <c r="R5" s="7" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="6" spans="2:17" ht="15.6">
+    <row r="6" spans="2:18" ht="15.6">
       <c r="B6" s="2" t="s">
         <v>3</v>
       </c>
@@ -938,23 +965,26 @@
         <v>50</v>
       </c>
       <c r="G6" s="5"/>
-      <c r="M6" s="7" t="s">
+      <c r="H6" s="12"/>
+      <c r="I6" s="12"/>
+      <c r="J6" s="13"/>
+      <c r="N6" s="7" t="s">
         <v>79</v>
       </c>
-      <c r="N6" t="s">
+      <c r="O6" t="s">
         <v>65</v>
       </c>
-      <c r="O6" s="8" t="s">
+      <c r="P6" s="8" t="s">
         <v>80</v>
       </c>
-      <c r="P6" t="s">
+      <c r="Q6" t="s">
         <v>67</v>
       </c>
-      <c r="Q6" s="7" t="s">
+      <c r="R6" s="7" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="7" spans="2:17" ht="15.6">
+    <row r="7" spans="2:18" ht="15.6">
       <c r="B7" s="2" t="s">
         <v>4</v>
       </c>
@@ -967,23 +997,26 @@
         <v>50</v>
       </c>
       <c r="G7" s="5"/>
-      <c r="M7" s="7" t="s">
+      <c r="H7" s="12"/>
+      <c r="I7" s="12"/>
+      <c r="J7" s="13"/>
+      <c r="N7" s="7" t="s">
         <v>79</v>
       </c>
-      <c r="N7" t="s">
+      <c r="O7" t="s">
         <v>68</v>
       </c>
-      <c r="O7" s="8" t="s">
+      <c r="P7" s="8" t="s">
         <v>80</v>
       </c>
-      <c r="P7" t="s">
+      <c r="Q7" t="s">
         <v>69</v>
       </c>
-      <c r="Q7" s="7" t="s">
+      <c r="R7" s="7" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="8" spans="2:17" ht="15.6">
+    <row r="8" spans="2:18" ht="15.6">
       <c r="B8" s="2" t="s">
         <v>5</v>
       </c>
@@ -994,23 +1027,26 @@
       <c r="G8" s="6" t="s">
         <v>49</v>
       </c>
-      <c r="M8" s="7" t="s">
+      <c r="H8" s="12"/>
+      <c r="I8" s="12"/>
+      <c r="J8" s="13"/>
+      <c r="N8" s="7" t="s">
         <v>79</v>
       </c>
-      <c r="N8" t="s">
+      <c r="O8" t="s">
         <v>70</v>
       </c>
-      <c r="O8" s="8" t="s">
+      <c r="P8" s="8" t="s">
         <v>80</v>
       </c>
-      <c r="P8" t="s">
+      <c r="Q8" t="s">
         <v>71</v>
       </c>
-      <c r="Q8" s="7" t="s">
+      <c r="R8" s="7" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="9" spans="2:17" ht="15.6">
+    <row r="9" spans="2:18" ht="15.6">
       <c r="B9" s="2" t="s">
         <v>6</v>
       </c>
@@ -1019,23 +1055,26 @@
       <c r="E9" s="5"/>
       <c r="F9" s="5"/>
       <c r="G9" s="5"/>
-      <c r="M9" s="7" t="s">
+      <c r="H9" s="12"/>
+      <c r="I9" s="12"/>
+      <c r="J9" s="13"/>
+      <c r="N9" s="7" t="s">
         <v>79</v>
       </c>
-      <c r="N9" t="s">
+      <c r="O9" t="s">
         <v>72</v>
       </c>
-      <c r="O9" s="8" t="s">
+      <c r="P9" s="8" t="s">
         <v>80</v>
       </c>
-      <c r="P9" t="s">
+      <c r="Q9" t="s">
         <v>73</v>
       </c>
-      <c r="Q9" s="7" t="s">
+      <c r="R9" s="7" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="10" spans="2:17" ht="15.6">
+    <row r="10" spans="2:18" ht="15.6">
       <c r="B10" s="2" t="s">
         <v>7</v>
       </c>
@@ -1046,24 +1085,27 @@
       <c r="G10" s="6" t="s">
         <v>49</v>
       </c>
-      <c r="J10" s="3"/>
-      <c r="M10" s="7" t="s">
+      <c r="H10" s="12"/>
+      <c r="I10" s="12"/>
+      <c r="J10" s="13"/>
+      <c r="K10" s="3"/>
+      <c r="N10" s="7" t="s">
         <v>79</v>
       </c>
-      <c r="N10" t="s">
+      <c r="O10" t="s">
         <v>74</v>
       </c>
-      <c r="O10" s="8" t="s">
+      <c r="P10" s="8" t="s">
         <v>80</v>
       </c>
-      <c r="P10" t="s">
+      <c r="Q10" t="s">
         <v>77</v>
       </c>
-      <c r="Q10" s="7" t="s">
+      <c r="R10" s="7" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="11" spans="2:17" ht="15.6">
+    <row r="11" spans="2:18" ht="15.6">
       <c r="B11" s="2" t="s">
         <v>8</v>
       </c>
@@ -1074,23 +1116,26 @@
       <c r="G11" s="6" t="s">
         <v>49</v>
       </c>
-      <c r="M11" s="7" t="s">
+      <c r="H11" s="12"/>
+      <c r="I11" s="12"/>
+      <c r="J11" s="13"/>
+      <c r="N11" s="7" t="s">
         <v>79</v>
       </c>
-      <c r="N11" t="s">
+      <c r="O11" t="s">
         <v>75</v>
       </c>
-      <c r="O11" s="8" t="s">
+      <c r="P11" s="8" t="s">
         <v>80</v>
       </c>
-      <c r="P11" t="s">
+      <c r="Q11" t="s">
         <v>76</v>
       </c>
-      <c r="Q11" s="7" t="s">
+      <c r="R11" s="7" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="12" spans="2:17" ht="15.6">
+    <row r="12" spans="2:18" ht="15.6">
       <c r="B12" s="2" t="s">
         <v>9</v>
       </c>
@@ -1103,11 +1148,13 @@
       <c r="G12" s="6" t="s">
         <v>49</v>
       </c>
-      <c r="I12" t="s">
+      <c r="H12" s="12"/>
+      <c r="I12" s="11" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="13" spans="2:17" ht="15.6">
+      <c r="J12" s="13"/>
+    </row>
+    <row r="13" spans="2:18" ht="15.6">
       <c r="B13" s="2" t="s">
         <v>10</v>
       </c>
@@ -1116,11 +1163,13 @@
       <c r="E13" s="5"/>
       <c r="F13" s="5"/>
       <c r="G13" s="5"/>
-      <c r="I13" t="s">
+      <c r="H13" s="12"/>
+      <c r="I13" s="11" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="14" spans="2:17" ht="15.6">
+      <c r="J13" s="13"/>
+    </row>
+    <row r="14" spans="2:18" ht="15.6">
       <c r="B14" s="2" t="s">
         <v>11</v>
       </c>
@@ -1133,26 +1182,28 @@
       <c r="G14" s="6" t="s">
         <v>49</v>
       </c>
-      <c r="I14" t="s">
+      <c r="H14" s="12"/>
+      <c r="I14" s="11" t="s">
         <v>57</v>
       </c>
-      <c r="M14" s="7" t="s">
+      <c r="J14" s="13"/>
+      <c r="N14" s="7" t="s">
         <v>79</v>
       </c>
-      <c r="N14" t="s">
+      <c r="O14" t="s">
         <v>58</v>
       </c>
-      <c r="O14" s="8" t="s">
+      <c r="P14" s="8" t="s">
         <v>80</v>
       </c>
-      <c r="P14" t="s">
+      <c r="Q14" t="s">
         <v>88</v>
       </c>
-      <c r="Q14" s="7" t="s">
+      <c r="R14" s="7" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="15" spans="2:17" ht="15.6">
+    <row r="15" spans="2:18" ht="15.6">
       <c r="B15" s="2" t="s">
         <v>12</v>
       </c>
@@ -1161,26 +1212,30 @@
       <c r="E15" s="5"/>
       <c r="F15" s="5"/>
       <c r="G15" s="5"/>
-      <c r="H15" t="s">
+      <c r="H15" s="11" t="s">
         <v>56</v>
       </c>
-      <c r="M15" s="7" t="s">
+      <c r="I15" s="12"/>
+      <c r="J15" s="13" t="s">
+        <v>100</v>
+      </c>
+      <c r="N15" s="7" t="s">
         <v>79</v>
       </c>
-      <c r="N15" t="s">
+      <c r="O15" t="s">
         <v>82</v>
       </c>
-      <c r="O15" s="8" t="s">
+      <c r="P15" s="8" t="s">
         <v>80</v>
       </c>
-      <c r="P15" t="s">
+      <c r="Q15" t="s">
         <v>89</v>
       </c>
-      <c r="Q15" s="7" t="s">
+      <c r="R15" s="7" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="16" spans="2:17" ht="15.6">
+    <row r="16" spans="2:18" ht="15.6">
       <c r="B16" s="2" t="s">
         <v>13</v>
       </c>
@@ -1189,26 +1244,30 @@
       <c r="E16" s="5"/>
       <c r="F16" s="5"/>
       <c r="G16" s="5"/>
-      <c r="H16" t="s">
+      <c r="H16" s="11" t="s">
         <v>56</v>
       </c>
-      <c r="M16" s="7" t="s">
+      <c r="I16" s="12"/>
+      <c r="J16" s="13" t="s">
+        <v>100</v>
+      </c>
+      <c r="N16" s="7" t="s">
         <v>79</v>
       </c>
-      <c r="N16" t="s">
+      <c r="O16" t="s">
         <v>83</v>
       </c>
-      <c r="O16" s="8" t="s">
+      <c r="P16" s="8" t="s">
         <v>80</v>
       </c>
-      <c r="P16" t="s">
+      <c r="Q16" t="s">
         <v>90</v>
       </c>
-      <c r="Q16" s="7" t="s">
+      <c r="R16" s="7" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="17" spans="2:17" ht="15.6">
+    <row r="17" spans="2:18" ht="15.6">
       <c r="B17" s="2" t="s">
         <v>14</v>
       </c>
@@ -1217,26 +1276,30 @@
       <c r="E17" s="5"/>
       <c r="F17" s="5"/>
       <c r="G17" s="5"/>
-      <c r="H17" t="s">
+      <c r="H17" s="11" t="s">
         <v>56</v>
       </c>
-      <c r="M17" s="7" t="s">
+      <c r="I17" s="12"/>
+      <c r="J17" s="13" t="s">
+        <v>100</v>
+      </c>
+      <c r="N17" s="7" t="s">
         <v>79</v>
       </c>
-      <c r="N17" t="s">
+      <c r="O17" t="s">
         <v>84</v>
       </c>
-      <c r="O17" s="8" t="s">
+      <c r="P17" s="8" t="s">
         <v>80</v>
       </c>
-      <c r="P17" t="s">
+      <c r="Q17" t="s">
         <v>91</v>
       </c>
-      <c r="Q17" s="7" t="s">
+      <c r="R17" s="7" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="18" spans="2:17" ht="15.6">
+    <row r="18" spans="2:18" ht="15.6">
       <c r="B18" s="2" t="s">
         <v>15</v>
       </c>
@@ -1245,23 +1308,26 @@
       <c r="E18" s="5"/>
       <c r="F18" s="5"/>
       <c r="G18" s="5"/>
-      <c r="M18" s="7" t="s">
+      <c r="H18" s="12"/>
+      <c r="I18" s="12"/>
+      <c r="J18" s="13"/>
+      <c r="N18" s="7" t="s">
         <v>79</v>
       </c>
-      <c r="N18" t="s">
+      <c r="O18" t="s">
         <v>85</v>
       </c>
-      <c r="O18" s="8" t="s">
+      <c r="P18" s="8" t="s">
         <v>80</v>
       </c>
-      <c r="P18" t="s">
+      <c r="Q18" t="s">
         <v>92</v>
       </c>
-      <c r="Q18" s="7" t="s">
+      <c r="R18" s="7" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="19" spans="2:17" ht="15.6">
+    <row r="19" spans="2:18" ht="15.6">
       <c r="B19" s="2" t="s">
         <v>16</v>
       </c>
@@ -1280,23 +1346,26 @@
       <c r="G19" s="6" t="s">
         <v>49</v>
       </c>
-      <c r="M19" s="7" t="s">
+      <c r="H19" s="12"/>
+      <c r="I19" s="12"/>
+      <c r="J19" s="13"/>
+      <c r="N19" s="7" t="s">
         <v>79</v>
       </c>
-      <c r="N19" t="s">
+      <c r="O19" t="s">
         <v>86</v>
       </c>
-      <c r="O19" s="8" t="s">
+      <c r="P19" s="8" t="s">
         <v>80</v>
       </c>
-      <c r="P19" t="s">
+      <c r="Q19" t="s">
         <v>93</v>
       </c>
-      <c r="Q19" s="7" t="s">
+      <c r="R19" s="7" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="20" spans="2:17" ht="15.6">
+    <row r="20" spans="2:18" ht="15.6">
       <c r="B20" s="2" t="s">
         <v>17</v>
       </c>
@@ -1315,23 +1384,26 @@
       <c r="G20" s="6" t="s">
         <v>49</v>
       </c>
-      <c r="M20" s="7" t="s">
+      <c r="H20" s="12"/>
+      <c r="I20" s="12"/>
+      <c r="J20" s="13"/>
+      <c r="N20" s="7" t="s">
         <v>79</v>
       </c>
-      <c r="N20" t="s">
+      <c r="O20" t="s">
         <v>87</v>
       </c>
-      <c r="O20" s="8" t="s">
+      <c r="P20" s="8" t="s">
         <v>80</v>
       </c>
-      <c r="P20" t="s">
+      <c r="Q20" t="s">
         <v>94</v>
       </c>
-      <c r="Q20" s="7" t="s">
+      <c r="R20" s="7" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="21" spans="2:17" ht="15.6">
+    <row r="21" spans="2:18" ht="15.6">
       <c r="B21" s="2" t="s">
         <v>18</v>
       </c>
@@ -1350,8 +1422,11 @@
       <c r="G21" s="6" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="22" spans="2:17" ht="15.6">
+      <c r="H21" s="12"/>
+      <c r="I21" s="12"/>
+      <c r="J21" s="13"/>
+    </row>
+    <row r="22" spans="2:18" ht="15.6">
       <c r="B22" s="2" t="s">
         <v>19</v>
       </c>
@@ -1364,16 +1439,19 @@
         <v>50</v>
       </c>
       <c r="G22" s="5"/>
-      <c r="L22" t="s">
+      <c r="H22" s="12"/>
+      <c r="I22" s="12"/>
+      <c r="J22" s="13"/>
+      <c r="M22" t="s">
         <v>95</v>
       </c>
-      <c r="M22" s="9" t="s">
+      <c r="N22" s="9" t="s">
         <v>96</v>
       </c>
-      <c r="O22" s="8"/>
-      <c r="Q22" s="7"/>
-    </row>
-    <row r="23" spans="2:17" ht="15.6">
+      <c r="P22" s="8"/>
+      <c r="R22" s="7"/>
+    </row>
+    <row r="23" spans="2:18" ht="15.6">
       <c r="B23" s="2" t="s">
         <v>20</v>
       </c>
@@ -1386,11 +1464,14 @@
         <v>50</v>
       </c>
       <c r="G23" s="5"/>
-      <c r="M23" s="7" t="s">
+      <c r="H23" s="12"/>
+      <c r="I23" s="12"/>
+      <c r="J23" s="13"/>
+      <c r="N23" s="7" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="24" spans="2:17" ht="15.6">
+    <row r="24" spans="2:18" ht="15.6">
       <c r="B24" s="2" t="s">
         <v>21</v>
       </c>
@@ -1403,11 +1484,14 @@
         <v>50</v>
       </c>
       <c r="G24" s="5"/>
-      <c r="M24" s="7" t="s">
+      <c r="H24" s="12"/>
+      <c r="I24" s="12"/>
+      <c r="J24" s="13"/>
+      <c r="N24" s="7" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="25" spans="2:17" ht="15.6">
+    <row r="25" spans="2:18" ht="15.6">
       <c r="B25" s="2" t="s">
         <v>22</v>
       </c>
@@ -1424,11 +1508,14 @@
         <v>50</v>
       </c>
       <c r="G25" s="5"/>
-      <c r="M25" s="9" t="s">
+      <c r="H25" s="12"/>
+      <c r="I25" s="12"/>
+      <c r="J25" s="13"/>
+      <c r="N25" s="9" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="26" spans="2:17" ht="15.6">
+    <row r="26" spans="2:18" ht="15.6">
       <c r="B26" s="2" t="s">
         <v>23</v>
       </c>
@@ -1439,11 +1526,13 @@
       <c r="G26" s="6" t="s">
         <v>49</v>
       </c>
-      <c r="I26" t="s">
+      <c r="H26" s="12"/>
+      <c r="I26" s="11" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="27" spans="2:17" ht="15.6">
+      <c r="J26" s="13"/>
+    </row>
+    <row r="27" spans="2:18" ht="15.6">
       <c r="B27" s="2" t="s">
         <v>24</v>
       </c>
@@ -1452,11 +1541,13 @@
       <c r="E27" s="5"/>
       <c r="F27" s="5"/>
       <c r="G27" s="5"/>
-      <c r="I27" t="s">
+      <c r="H27" s="12"/>
+      <c r="I27" s="11" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="28" spans="2:17" ht="15.6">
+      <c r="J27" s="13"/>
+    </row>
+    <row r="28" spans="2:18" ht="15.6">
       <c r="B28" s="2" t="s">
         <v>25</v>
       </c>
@@ -1467,11 +1558,13 @@
       <c r="G28" s="6" t="s">
         <v>49</v>
       </c>
-      <c r="I28" t="s">
+      <c r="H28" s="12"/>
+      <c r="I28" s="11" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="29" spans="2:17" ht="15.6">
+      <c r="J28" s="13"/>
+    </row>
+    <row r="29" spans="2:18" ht="15.6">
       <c r="B29" s="2" t="s">
         <v>26</v>
       </c>
@@ -1482,11 +1575,13 @@
       <c r="G29" s="6" t="s">
         <v>49</v>
       </c>
-      <c r="I29" t="s">
+      <c r="H29" s="12"/>
+      <c r="I29" s="11" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="30" spans="2:17" ht="15.6">
+      <c r="J29" s="13"/>
+    </row>
+    <row r="30" spans="2:18" ht="15.6">
       <c r="B30" s="2" t="s">
         <v>27</v>
       </c>
@@ -1497,11 +1592,15 @@
       </c>
       <c r="F30" s="5"/>
       <c r="G30" s="5"/>
-      <c r="H30" t="s">
+      <c r="H30" s="11" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="31" spans="2:17" ht="15.6">
+      <c r="I30" s="12"/>
+      <c r="J30" s="13" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="31" spans="2:18" ht="15.6">
       <c r="B31" s="2" t="s">
         <v>28</v>
       </c>
@@ -1512,11 +1611,15 @@
       </c>
       <c r="F31" s="5"/>
       <c r="G31" s="5"/>
-      <c r="H31" t="s">
+      <c r="H31" s="11" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="32" spans="2:17" ht="15.6">
+      <c r="I31" s="12"/>
+      <c r="J31" s="13" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="32" spans="2:18" ht="15.6">
       <c r="B32" s="2" t="s">
         <v>29</v>
       </c>
@@ -1527,11 +1630,15 @@
       </c>
       <c r="F32" s="5"/>
       <c r="G32" s="5"/>
-      <c r="H32" t="s">
+      <c r="H32" s="11" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="33" spans="2:8" ht="15.6">
+      <c r="I32" s="12"/>
+      <c r="J32" s="13" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="33" spans="2:10" ht="15.6">
       <c r="B33" s="2" t="s">
         <v>30</v>
       </c>
@@ -1542,11 +1649,15 @@
       </c>
       <c r="F33" s="5"/>
       <c r="G33" s="5"/>
-      <c r="H33" t="s">
+      <c r="H33" s="11" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="34" spans="2:8" ht="15.6">
+      <c r="I33" s="12"/>
+      <c r="J33" s="13" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="34" spans="2:10" ht="15.6">
       <c r="B34" s="2" t="s">
         <v>31</v>
       </c>
@@ -1557,11 +1668,13 @@
       </c>
       <c r="F34" s="5"/>
       <c r="G34" s="5"/>
-      <c r="H34" t="s">
+      <c r="H34" s="11" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="35" spans="2:8" ht="15.6">
+      <c r="I34" s="12"/>
+      <c r="J34" s="13"/>
+    </row>
+    <row r="35" spans="2:10" ht="15.6">
       <c r="B35" s="2" t="s">
         <v>32</v>
       </c>
@@ -1574,8 +1687,11 @@
         <v>50</v>
       </c>
       <c r="G35" s="5"/>
-    </row>
-    <row r="36" spans="2:8" ht="15.6">
+      <c r="H35" s="12"/>
+      <c r="I35" s="12"/>
+      <c r="J35" s="13"/>
+    </row>
+    <row r="36" spans="2:10" ht="15.6">
       <c r="B36" s="2" t="s">
         <v>33</v>
       </c>
@@ -1588,8 +1704,11 @@
         <v>50</v>
       </c>
       <c r="G36" s="5"/>
-    </row>
-    <row r="37" spans="2:8" ht="15.6">
+      <c r="H36" s="12"/>
+      <c r="I36" s="12"/>
+      <c r="J36" s="13"/>
+    </row>
+    <row r="37" spans="2:10" ht="15.6">
       <c r="B37" s="2" t="s">
         <v>34</v>
       </c>
@@ -1602,8 +1721,11 @@
         <v>50</v>
       </c>
       <c r="G37" s="5"/>
-    </row>
-    <row r="38" spans="2:8" ht="15.6">
+      <c r="H37" s="12"/>
+      <c r="I37" s="12"/>
+      <c r="J37" s="13"/>
+    </row>
+    <row r="38" spans="2:10" ht="15.6">
       <c r="B38" s="2" t="s">
         <v>35</v>
       </c>
@@ -1616,8 +1738,11 @@
         <v>50</v>
       </c>
       <c r="G38" s="5"/>
-    </row>
-    <row r="39" spans="2:8" ht="15.6">
+      <c r="H38" s="12"/>
+      <c r="I38" s="12"/>
+      <c r="J38" s="13"/>
+    </row>
+    <row r="39" spans="2:10" ht="15.6">
       <c r="B39" s="2" t="s">
         <v>36</v>
       </c>
@@ -1628,8 +1753,11 @@
       <c r="G39" s="6" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="40" spans="2:8" ht="15.6">
+      <c r="H39" s="12"/>
+      <c r="I39" s="12"/>
+      <c r="J39" s="13"/>
+    </row>
+    <row r="40" spans="2:10" ht="15.6">
       <c r="B40" s="2" t="s">
         <v>37</v>
       </c>
@@ -1638,8 +1766,11 @@
       <c r="E40" s="5"/>
       <c r="F40" s="5"/>
       <c r="G40" s="5"/>
-    </row>
-    <row r="41" spans="2:8" ht="15.6">
+      <c r="H40" s="12"/>
+      <c r="I40" s="12"/>
+      <c r="J40" s="13"/>
+    </row>
+    <row r="41" spans="2:10" ht="15.6">
       <c r="B41" s="2" t="s">
         <v>38</v>
       </c>
@@ -1650,8 +1781,11 @@
       <c r="G41" s="6" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="42" spans="2:8" ht="15.6">
+      <c r="H41" s="12"/>
+      <c r="I41" s="12"/>
+      <c r="J41" s="13"/>
+    </row>
+    <row r="42" spans="2:10" ht="15.6">
       <c r="B42" s="2" t="s">
         <v>39</v>
       </c>
@@ -1662,8 +1796,11 @@
       </c>
       <c r="F42" s="5"/>
       <c r="G42" s="5"/>
-    </row>
-    <row r="43" spans="2:8" ht="15.6">
+      <c r="H42" s="12"/>
+      <c r="I42" s="12"/>
+      <c r="J42" s="13"/>
+    </row>
+    <row r="43" spans="2:10" ht="15.6">
       <c r="B43" s="2" t="s">
         <v>40</v>
       </c>
@@ -1674,8 +1811,13 @@
       </c>
       <c r="F43" s="5"/>
       <c r="G43" s="5"/>
-    </row>
-    <row r="44" spans="2:8" ht="15.6">
+      <c r="H43" s="12"/>
+      <c r="I43" s="12"/>
+      <c r="J43" s="13" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="44" spans="2:10" ht="15.6">
       <c r="B44" s="2" t="s">
         <v>41</v>
       </c>
@@ -1684,8 +1826,13 @@
       <c r="E44" s="5"/>
       <c r="F44" s="5"/>
       <c r="G44" s="5"/>
-    </row>
-    <row r="45" spans="2:8" ht="15.6">
+      <c r="H44" s="12"/>
+      <c r="I44" s="12"/>
+      <c r="J44" s="13" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="45" spans="2:10" ht="15.6">
       <c r="B45" s="2" t="s">
         <v>42</v>
       </c>
@@ -1696,8 +1843,13 @@
       </c>
       <c r="F45" s="5"/>
       <c r="G45" s="5"/>
-    </row>
-    <row r="46" spans="2:8" ht="15.6">
+      <c r="H45" s="12"/>
+      <c r="I45" s="12"/>
+      <c r="J45" s="13" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="46" spans="2:10" ht="15.6">
       <c r="B46" s="2" t="s">
         <v>43</v>
       </c>
@@ -1708,6 +1860,11 @@
       </c>
       <c r="F46" s="5"/>
       <c r="G46" s="5"/>
+      <c r="H46" s="12"/>
+      <c r="I46" s="12"/>
+      <c r="J46" s="13" t="s">
+        <v>100</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Added view to entered results
</commit_message>
<xml_diff>
--- a/Role permissions.xlsx
+++ b/Role permissions.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21328"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6609DC37-178D-471C-98B1-B728D0B15541}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D2561D40-D49C-44AF-84F3-431E33C827D8}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="916" uniqueCount="101">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="235" uniqueCount="101">
   <si>
     <t>/compound/add [GET]</t>
   </si>
@@ -794,8 +794,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B2:R46"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J43" sqref="J43:J46"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="B22" sqref="B22:F22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -1141,9 +1141,7 @@
       </c>
       <c r="C12" s="5"/>
       <c r="D12" s="5"/>
-      <c r="E12" s="6" t="s">
-        <v>52</v>
-      </c>
+      <c r="E12" s="5"/>
       <c r="F12" s="5"/>
       <c r="G12" s="6" t="s">
         <v>49</v>
@@ -1175,9 +1173,7 @@
       </c>
       <c r="C14" s="5"/>
       <c r="D14" s="5"/>
-      <c r="E14" s="6" t="s">
-        <v>52</v>
-      </c>
+      <c r="E14" s="5"/>
       <c r="F14" s="5"/>
       <c r="G14" s="6" t="s">
         <v>49</v>
@@ -1796,7 +1792,9 @@
       </c>
       <c r="F42" s="5"/>
       <c r="G42" s="5"/>
-      <c r="H42" s="12"/>
+      <c r="H42" s="11" t="s">
+        <v>56</v>
+      </c>
       <c r="I42" s="12"/>
       <c r="J42" s="13"/>
     </row>
@@ -1811,7 +1809,9 @@
       </c>
       <c r="F43" s="5"/>
       <c r="G43" s="5"/>
-      <c r="H43" s="12"/>
+      <c r="H43" s="11" t="s">
+        <v>56</v>
+      </c>
       <c r="I43" s="12"/>
       <c r="J43" s="13" t="s">
         <v>100</v>
@@ -1826,7 +1826,9 @@
       <c r="E44" s="5"/>
       <c r="F44" s="5"/>
       <c r="G44" s="5"/>
-      <c r="H44" s="12"/>
+      <c r="H44" s="11" t="s">
+        <v>56</v>
+      </c>
       <c r="I44" s="12"/>
       <c r="J44" s="13" t="s">
         <v>100</v>
@@ -1843,7 +1845,9 @@
       </c>
       <c r="F45" s="5"/>
       <c r="G45" s="5"/>
-      <c r="H45" s="12"/>
+      <c r="H45" s="11" t="s">
+        <v>56</v>
+      </c>
       <c r="I45" s="12"/>
       <c r="J45" s="13" t="s">
         <v>100</v>
@@ -1860,7 +1864,9 @@
       </c>
       <c r="F46" s="5"/>
       <c r="G46" s="5"/>
-      <c r="H46" s="12"/>
+      <c r="H46" s="11" t="s">
+        <v>56</v>
+      </c>
       <c r="I46" s="12"/>
       <c r="J46" s="13" t="s">
         <v>100</v>

</xml_diff>

<commit_message>
Compound frontend changed. User frontend changed. Security added in mainWindow.html
</commit_message>
<xml_diff>
--- a/Role permissions.xlsx
+++ b/Role permissions.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21328"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D2561D40-D49C-44AF-84F3-431E33C827D8}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5317565D-C43E-4E9E-8ECD-403EBE5314B7}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="235" uniqueCount="101">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="240" uniqueCount="101">
   <si>
     <t>/compound/add [GET]</t>
   </si>
@@ -472,7 +472,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -503,6 +503,16 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -792,10 +802,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B2:R46"/>
+  <dimension ref="B2:R54"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="B22" sqref="B22:F22"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K21" sqref="K21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -1017,44 +1027,30 @@
       </c>
     </row>
     <row r="8" spans="2:18" ht="15.6">
-      <c r="B8" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C8" s="5"/>
-      <c r="D8" s="5"/>
-      <c r="E8" s="5"/>
-      <c r="F8" s="5"/>
-      <c r="G8" s="6" t="s">
-        <v>49</v>
-      </c>
-      <c r="H8" s="12"/>
-      <c r="I8" s="12"/>
+      <c r="B8" s="13"/>
+      <c r="C8" s="14"/>
+      <c r="D8" s="14"/>
+      <c r="E8" s="14"/>
+      <c r="F8" s="14"/>
+      <c r="G8" s="14"/>
+      <c r="H8" s="13"/>
+      <c r="I8" s="13"/>
       <c r="J8" s="13"/>
-      <c r="N8" s="7" t="s">
-        <v>79</v>
-      </c>
-      <c r="O8" t="s">
-        <v>70</v>
-      </c>
-      <c r="P8" s="8" t="s">
-        <v>80</v>
-      </c>
-      <c r="Q8" t="s">
-        <v>71</v>
-      </c>
-      <c r="R8" s="7" t="s">
-        <v>81</v>
-      </c>
+      <c r="N8" s="7"/>
+      <c r="P8" s="8"/>
+      <c r="R8" s="7"/>
     </row>
     <row r="9" spans="2:18" ht="15.6">
       <c r="B9" s="2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C9" s="5"/>
       <c r="D9" s="5"/>
       <c r="E9" s="5"/>
       <c r="F9" s="5"/>
-      <c r="G9" s="5"/>
+      <c r="G9" s="6" t="s">
+        <v>49</v>
+      </c>
       <c r="H9" s="12"/>
       <c r="I9" s="12"/>
       <c r="J9" s="13"/>
@@ -1062,13 +1058,13 @@
         <v>79</v>
       </c>
       <c r="O9" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="P9" s="8" t="s">
         <v>80</v>
       </c>
       <c r="Q9" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="R9" s="7" t="s">
         <v>81</v>
@@ -1076,30 +1072,27 @@
     </row>
     <row r="10" spans="2:18" ht="15.6">
       <c r="B10" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C10" s="5"/>
       <c r="D10" s="5"/>
       <c r="E10" s="5"/>
       <c r="F10" s="5"/>
-      <c r="G10" s="6" t="s">
-        <v>49</v>
-      </c>
+      <c r="G10" s="5"/>
       <c r="H10" s="12"/>
       <c r="I10" s="12"/>
       <c r="J10" s="13"/>
-      <c r="K10" s="3"/>
       <c r="N10" s="7" t="s">
         <v>79</v>
       </c>
       <c r="O10" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="P10" s="8" t="s">
         <v>80</v>
       </c>
       <c r="Q10" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="R10" s="7" t="s">
         <v>81</v>
@@ -1107,7 +1100,7 @@
     </row>
     <row r="11" spans="2:18" ht="15.6">
       <c r="B11" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C11" s="5"/>
       <c r="D11" s="5"/>
@@ -1119,17 +1112,18 @@
       <c r="H11" s="12"/>
       <c r="I11" s="12"/>
       <c r="J11" s="13"/>
+      <c r="K11" s="3"/>
       <c r="N11" s="7" t="s">
         <v>79</v>
       </c>
       <c r="O11" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="P11" s="8" t="s">
         <v>80</v>
       </c>
       <c r="Q11" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="R11" s="7" t="s">
         <v>81</v>
@@ -1137,7 +1131,7 @@
     </row>
     <row r="12" spans="2:18" ht="15.6">
       <c r="B12" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C12" s="5"/>
       <c r="D12" s="5"/>
@@ -1147,29 +1141,41 @@
         <v>49</v>
       </c>
       <c r="H12" s="12"/>
-      <c r="I12" s="11" t="s">
-        <v>57</v>
-      </c>
+      <c r="I12" s="12"/>
       <c r="J12" s="13"/>
-    </row>
-    <row r="13" spans="2:18" ht="15.6">
-      <c r="B13" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="C13" s="5"/>
-      <c r="D13" s="5"/>
-      <c r="E13" s="5"/>
-      <c r="F13" s="5"/>
-      <c r="G13" s="5"/>
-      <c r="H13" s="12"/>
-      <c r="I13" s="11" t="s">
-        <v>57</v>
-      </c>
+      <c r="N12" s="7" t="s">
+        <v>79</v>
+      </c>
+      <c r="O12" t="s">
+        <v>75</v>
+      </c>
+      <c r="P12" s="8" t="s">
+        <v>80</v>
+      </c>
+      <c r="Q12" t="s">
+        <v>76</v>
+      </c>
+      <c r="R12" s="7" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="13" spans="2:18" s="15" customFormat="1" ht="15.6">
+      <c r="B13" s="13"/>
+      <c r="C13" s="14"/>
+      <c r="D13" s="14"/>
+      <c r="E13" s="14"/>
+      <c r="F13" s="14"/>
+      <c r="G13" s="14"/>
+      <c r="H13" s="13"/>
+      <c r="I13" s="13"/>
       <c r="J13" s="13"/>
+      <c r="N13" s="16"/>
+      <c r="P13" s="17"/>
+      <c r="R13" s="16"/>
     </row>
     <row r="14" spans="2:18" ht="15.6">
       <c r="B14" s="2" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C14" s="5"/>
       <c r="D14" s="5"/>
@@ -1183,141 +1189,95 @@
         <v>57</v>
       </c>
       <c r="J14" s="13"/>
-      <c r="N14" s="7" t="s">
-        <v>79</v>
-      </c>
-      <c r="O14" t="s">
-        <v>58</v>
-      </c>
-      <c r="P14" s="8" t="s">
-        <v>80</v>
-      </c>
-      <c r="Q14" t="s">
-        <v>88</v>
-      </c>
-      <c r="R14" s="7" t="s">
-        <v>81</v>
-      </c>
     </row>
     <row r="15" spans="2:18" ht="15.6">
       <c r="B15" s="2" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="C15" s="5"/>
       <c r="D15" s="5"/>
       <c r="E15" s="5"/>
       <c r="F15" s="5"/>
       <c r="G15" s="5"/>
-      <c r="H15" s="11" t="s">
-        <v>56</v>
-      </c>
-      <c r="I15" s="12"/>
-      <c r="J15" s="13" t="s">
-        <v>100</v>
-      </c>
-      <c r="N15" s="7" t="s">
-        <v>79</v>
-      </c>
-      <c r="O15" t="s">
-        <v>82</v>
-      </c>
-      <c r="P15" s="8" t="s">
-        <v>80</v>
-      </c>
-      <c r="Q15" t="s">
-        <v>89</v>
-      </c>
-      <c r="R15" s="7" t="s">
-        <v>81</v>
-      </c>
+      <c r="H15" s="12"/>
+      <c r="I15" s="11" t="s">
+        <v>57</v>
+      </c>
+      <c r="J15" s="13"/>
     </row>
     <row r="16" spans="2:18" ht="15.6">
       <c r="B16" s="2" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="C16" s="5"/>
       <c r="D16" s="5"/>
       <c r="E16" s="5"/>
       <c r="F16" s="5"/>
-      <c r="G16" s="5"/>
-      <c r="H16" s="11" t="s">
-        <v>56</v>
-      </c>
-      <c r="I16" s="12"/>
-      <c r="J16" s="13" t="s">
-        <v>100</v>
-      </c>
+      <c r="G16" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="H16" s="12"/>
+      <c r="I16" s="11" t="s">
+        <v>57</v>
+      </c>
+      <c r="J16" s="13"/>
       <c r="N16" s="7" t="s">
         <v>79</v>
       </c>
       <c r="O16" t="s">
-        <v>83</v>
+        <v>58</v>
       </c>
       <c r="P16" s="8" t="s">
         <v>80</v>
       </c>
       <c r="Q16" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="R16" s="7" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="17" spans="2:18" ht="15.6">
-      <c r="B17" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="C17" s="5"/>
-      <c r="D17" s="5"/>
-      <c r="E17" s="5"/>
-      <c r="F17" s="5"/>
-      <c r="G17" s="5"/>
-      <c r="H17" s="11" t="s">
-        <v>56</v>
-      </c>
-      <c r="I17" s="12"/>
-      <c r="J17" s="13" t="s">
-        <v>100</v>
-      </c>
-      <c r="N17" s="7" t="s">
-        <v>79</v>
-      </c>
-      <c r="O17" t="s">
-        <v>84</v>
-      </c>
-      <c r="P17" s="8" t="s">
-        <v>80</v>
-      </c>
-      <c r="Q17" t="s">
-        <v>91</v>
-      </c>
-      <c r="R17" s="7" t="s">
-        <v>81</v>
-      </c>
+    <row r="17" spans="2:18" s="15" customFormat="1" ht="15.6">
+      <c r="B17" s="13"/>
+      <c r="C17" s="14"/>
+      <c r="D17" s="14"/>
+      <c r="E17" s="14"/>
+      <c r="F17" s="14"/>
+      <c r="G17" s="14"/>
+      <c r="H17" s="13"/>
+      <c r="I17" s="13"/>
+      <c r="J17" s="13"/>
+      <c r="N17" s="16"/>
+      <c r="P17" s="17"/>
+      <c r="R17" s="16"/>
     </row>
     <row r="18" spans="2:18" ht="15.6">
       <c r="B18" s="2" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="C18" s="5"/>
       <c r="D18" s="5"/>
       <c r="E18" s="5"/>
       <c r="F18" s="5"/>
       <c r="G18" s="5"/>
-      <c r="H18" s="12"/>
+      <c r="H18" s="11" t="s">
+        <v>56</v>
+      </c>
       <c r="I18" s="12"/>
-      <c r="J18" s="13"/>
+      <c r="J18" s="13" t="s">
+        <v>100</v>
+      </c>
       <c r="N18" s="7" t="s">
         <v>79</v>
       </c>
       <c r="O18" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="P18" s="8" t="s">
         <v>80</v>
       </c>
       <c r="Q18" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="R18" s="7" t="s">
         <v>81</v>
@@ -1325,37 +1285,31 @@
     </row>
     <row r="19" spans="2:18" ht="15.6">
       <c r="B19" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="C19" s="6" t="s">
-        <v>48</v>
-      </c>
-      <c r="D19" s="6" t="s">
-        <v>53</v>
-      </c>
-      <c r="E19" s="6" t="s">
-        <v>52</v>
-      </c>
-      <c r="F19" s="6" t="s">
-        <v>50</v>
-      </c>
-      <c r="G19" s="6" t="s">
-        <v>49</v>
-      </c>
-      <c r="H19" s="12"/>
+        <v>13</v>
+      </c>
+      <c r="C19" s="5"/>
+      <c r="D19" s="5"/>
+      <c r="E19" s="5"/>
+      <c r="F19" s="5"/>
+      <c r="G19" s="5"/>
+      <c r="H19" s="11" t="s">
+        <v>56</v>
+      </c>
       <c r="I19" s="12"/>
-      <c r="J19" s="13"/>
+      <c r="J19" s="13" t="s">
+        <v>100</v>
+      </c>
       <c r="N19" s="7" t="s">
         <v>79</v>
       </c>
       <c r="O19" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="P19" s="8" t="s">
         <v>80</v>
       </c>
       <c r="Q19" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="R19" s="7" t="s">
         <v>81</v>
@@ -1363,37 +1317,31 @@
     </row>
     <row r="20" spans="2:18" ht="15.6">
       <c r="B20" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="C20" s="6" t="s">
-        <v>48</v>
-      </c>
-      <c r="D20" s="6" t="s">
-        <v>53</v>
-      </c>
-      <c r="E20" s="6" t="s">
-        <v>52</v>
-      </c>
-      <c r="F20" s="6" t="s">
-        <v>50</v>
-      </c>
-      <c r="G20" s="6" t="s">
-        <v>49</v>
-      </c>
-      <c r="H20" s="12"/>
+        <v>14</v>
+      </c>
+      <c r="C20" s="5"/>
+      <c r="D20" s="5"/>
+      <c r="E20" s="5"/>
+      <c r="F20" s="5"/>
+      <c r="G20" s="5"/>
+      <c r="H20" s="11" t="s">
+        <v>56</v>
+      </c>
       <c r="I20" s="12"/>
-      <c r="J20" s="13"/>
+      <c r="J20" s="13" t="s">
+        <v>100</v>
+      </c>
       <c r="N20" s="7" t="s">
         <v>79</v>
       </c>
       <c r="O20" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="P20" s="8" t="s">
         <v>80</v>
       </c>
       <c r="Q20" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="R20" s="7" t="s">
         <v>81</v>
@@ -1401,474 +1349,644 @@
     </row>
     <row r="21" spans="2:18" ht="15.6">
       <c r="B21" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="C21" s="6" t="s">
-        <v>48</v>
-      </c>
-      <c r="D21" s="6" t="s">
-        <v>53</v>
-      </c>
-      <c r="E21" s="6" t="s">
-        <v>52</v>
-      </c>
-      <c r="F21" s="6" t="s">
-        <v>50</v>
-      </c>
-      <c r="G21" s="6" t="s">
-        <v>49</v>
-      </c>
-      <c r="H21" s="12"/>
+        <v>15</v>
+      </c>
+      <c r="C21" s="5"/>
+      <c r="D21" s="5"/>
+      <c r="E21" s="5"/>
+      <c r="F21" s="5"/>
+      <c r="G21" s="5"/>
+      <c r="H21" s="11" t="s">
+        <v>56</v>
+      </c>
       <c r="I21" s="12"/>
-      <c r="J21" s="13"/>
+      <c r="J21" s="13" t="s">
+        <v>100</v>
+      </c>
+      <c r="N21" s="7" t="s">
+        <v>79</v>
+      </c>
+      <c r="O21" t="s">
+        <v>85</v>
+      </c>
+      <c r="P21" s="8" t="s">
+        <v>80</v>
+      </c>
+      <c r="Q21" t="s">
+        <v>92</v>
+      </c>
+      <c r="R21" s="7" t="s">
+        <v>81</v>
+      </c>
     </row>
     <row r="22" spans="2:18" ht="15.6">
       <c r="B22" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="C22" s="5"/>
-      <c r="D22" s="5"/>
+        <v>16</v>
+      </c>
+      <c r="C22" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="D22" s="6" t="s">
+        <v>53</v>
+      </c>
       <c r="E22" s="6" t="s">
         <v>52</v>
       </c>
       <c r="F22" s="6" t="s">
         <v>50</v>
       </c>
-      <c r="G22" s="5"/>
+      <c r="G22" s="6" t="s">
+        <v>49</v>
+      </c>
       <c r="H22" s="12"/>
       <c r="I22" s="12"/>
-      <c r="J22" s="13"/>
-      <c r="M22" t="s">
-        <v>95</v>
-      </c>
-      <c r="N22" s="9" t="s">
-        <v>96</v>
-      </c>
-      <c r="P22" s="8"/>
-      <c r="R22" s="7"/>
+      <c r="J22" s="13" t="s">
+        <v>100</v>
+      </c>
+      <c r="N22" s="7" t="s">
+        <v>79</v>
+      </c>
+      <c r="O22" t="s">
+        <v>86</v>
+      </c>
+      <c r="P22" s="8" t="s">
+        <v>80</v>
+      </c>
+      <c r="Q22" t="s">
+        <v>93</v>
+      </c>
+      <c r="R22" s="7" t="s">
+        <v>81</v>
+      </c>
     </row>
     <row r="23" spans="2:18" ht="15.6">
       <c r="B23" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="C23" s="5"/>
-      <c r="D23" s="5"/>
+        <v>17</v>
+      </c>
+      <c r="C23" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="D23" s="6" t="s">
+        <v>53</v>
+      </c>
       <c r="E23" s="6" t="s">
         <v>52</v>
       </c>
       <c r="F23" s="6" t="s">
         <v>50</v>
       </c>
-      <c r="G23" s="5"/>
+      <c r="G23" s="6" t="s">
+        <v>49</v>
+      </c>
       <c r="H23" s="12"/>
       <c r="I23" s="12"/>
-      <c r="J23" s="13"/>
+      <c r="J23" s="13" t="s">
+        <v>100</v>
+      </c>
       <c r="N23" s="7" t="s">
-        <v>97</v>
+        <v>79</v>
+      </c>
+      <c r="O23" t="s">
+        <v>87</v>
+      </c>
+      <c r="P23" s="8" t="s">
+        <v>80</v>
+      </c>
+      <c r="Q23" t="s">
+        <v>94</v>
+      </c>
+      <c r="R23" s="7" t="s">
+        <v>81</v>
       </c>
     </row>
     <row r="24" spans="2:18" ht="15.6">
       <c r="B24" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="C24" s="5"/>
-      <c r="D24" s="5"/>
+        <v>18</v>
+      </c>
+      <c r="C24" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="D24" s="6" t="s">
+        <v>53</v>
+      </c>
       <c r="E24" s="6" t="s">
         <v>52</v>
       </c>
       <c r="F24" s="6" t="s">
         <v>50</v>
       </c>
-      <c r="G24" s="5"/>
+      <c r="G24" s="6" t="s">
+        <v>49</v>
+      </c>
       <c r="H24" s="12"/>
       <c r="I24" s="12"/>
-      <c r="J24" s="13"/>
-      <c r="N24" s="7" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="25" spans="2:18" ht="15.6">
-      <c r="B25" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="C25" s="6" t="s">
-        <v>48</v>
-      </c>
-      <c r="D25" s="6" t="s">
-        <v>53</v>
-      </c>
-      <c r="E25" s="6" t="s">
-        <v>52</v>
-      </c>
-      <c r="F25" s="6" t="s">
-        <v>50</v>
-      </c>
-      <c r="G25" s="5"/>
-      <c r="H25" s="12"/>
-      <c r="I25" s="12"/>
+      <c r="J24" s="13" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="25" spans="2:18" s="15" customFormat="1" ht="15.6">
+      <c r="B25" s="13"/>
+      <c r="C25" s="14"/>
+      <c r="D25" s="14"/>
+      <c r="E25" s="14"/>
+      <c r="F25" s="14"/>
+      <c r="G25" s="14"/>
+      <c r="H25" s="13"/>
+      <c r="I25" s="13"/>
       <c r="J25" s="13"/>
-      <c r="N25" s="9" t="s">
-        <v>99</v>
-      </c>
     </row>
     <row r="26" spans="2:18" ht="15.6">
       <c r="B26" s="2" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="C26" s="5"/>
       <c r="D26" s="5"/>
-      <c r="E26" s="5"/>
-      <c r="F26" s="5"/>
-      <c r="G26" s="6" t="s">
-        <v>49</v>
-      </c>
+      <c r="E26" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="F26" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="G26" s="5"/>
       <c r="H26" s="12"/>
-      <c r="I26" s="11" t="s">
-        <v>57</v>
-      </c>
+      <c r="I26" s="12"/>
       <c r="J26" s="13"/>
+      <c r="M26" t="s">
+        <v>95</v>
+      </c>
+      <c r="N26" s="9" t="s">
+        <v>96</v>
+      </c>
+      <c r="P26" s="8"/>
+      <c r="R26" s="7"/>
     </row>
     <row r="27" spans="2:18" ht="15.6">
       <c r="B27" s="2" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="C27" s="5"/>
       <c r="D27" s="5"/>
-      <c r="E27" s="5"/>
-      <c r="F27" s="5"/>
+      <c r="E27" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="F27" s="6" t="s">
+        <v>50</v>
+      </c>
       <c r="G27" s="5"/>
       <c r="H27" s="12"/>
-      <c r="I27" s="11" t="s">
-        <v>57</v>
-      </c>
+      <c r="I27" s="12"/>
       <c r="J27" s="13"/>
+      <c r="N27" s="7" t="s">
+        <v>97</v>
+      </c>
     </row>
     <row r="28" spans="2:18" ht="15.6">
       <c r="B28" s="2" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="C28" s="5"/>
       <c r="D28" s="5"/>
-      <c r="E28" s="5"/>
-      <c r="F28" s="5"/>
-      <c r="G28" s="6" t="s">
-        <v>49</v>
-      </c>
+      <c r="E28" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="F28" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="G28" s="5"/>
       <c r="H28" s="12"/>
-      <c r="I28" s="11" t="s">
-        <v>57</v>
-      </c>
+      <c r="I28" s="12"/>
       <c r="J28" s="13"/>
+      <c r="N28" s="7" t="s">
+        <v>98</v>
+      </c>
     </row>
     <row r="29" spans="2:18" ht="15.6">
       <c r="B29" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="C29" s="5"/>
-      <c r="D29" s="5"/>
-      <c r="E29" s="5"/>
-      <c r="F29" s="5"/>
-      <c r="G29" s="6" t="s">
-        <v>49</v>
-      </c>
+        <v>22</v>
+      </c>
+      <c r="C29" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="D29" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="E29" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="F29" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="G29" s="5"/>
       <c r="H29" s="12"/>
-      <c r="I29" s="11" t="s">
-        <v>57</v>
-      </c>
+      <c r="I29" s="12"/>
       <c r="J29" s="13"/>
-    </row>
-    <row r="30" spans="2:18" ht="15.6">
-      <c r="B30" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="C30" s="5"/>
-      <c r="D30" s="5"/>
-      <c r="E30" s="6" t="s">
-        <v>52</v>
-      </c>
-      <c r="F30" s="5"/>
-      <c r="G30" s="5"/>
-      <c r="H30" s="11" t="s">
-        <v>56</v>
-      </c>
-      <c r="I30" s="12"/>
-      <c r="J30" s="13" t="s">
-        <v>100</v>
-      </c>
+      <c r="N29" s="9" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="30" spans="2:18" s="15" customFormat="1" ht="15.6">
+      <c r="B30" s="13"/>
+      <c r="C30" s="14"/>
+      <c r="D30" s="14"/>
+      <c r="E30" s="14"/>
+      <c r="F30" s="14"/>
+      <c r="G30" s="14"/>
+      <c r="H30" s="13"/>
+      <c r="I30" s="13"/>
+      <c r="J30" s="13"/>
+      <c r="N30" s="16"/>
     </row>
     <row r="31" spans="2:18" ht="15.6">
       <c r="B31" s="2" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="C31" s="5"/>
       <c r="D31" s="5"/>
-      <c r="E31" s="6" t="s">
-        <v>52</v>
-      </c>
+      <c r="E31" s="5"/>
       <c r="F31" s="5"/>
-      <c r="G31" s="5"/>
-      <c r="H31" s="11" t="s">
-        <v>56</v>
-      </c>
-      <c r="I31" s="12"/>
-      <c r="J31" s="13" t="s">
-        <v>100</v>
-      </c>
+      <c r="G31" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="H31" s="12"/>
+      <c r="I31" s="11" t="s">
+        <v>57</v>
+      </c>
+      <c r="J31" s="13"/>
     </row>
     <row r="32" spans="2:18" ht="15.6">
       <c r="B32" s="2" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
       <c r="C32" s="5"/>
       <c r="D32" s="5"/>
-      <c r="E32" s="6" t="s">
-        <v>52</v>
-      </c>
+      <c r="E32" s="5"/>
       <c r="F32" s="5"/>
       <c r="G32" s="5"/>
-      <c r="H32" s="11" t="s">
-        <v>56</v>
-      </c>
-      <c r="I32" s="12"/>
-      <c r="J32" s="13" t="s">
-        <v>100</v>
-      </c>
+      <c r="H32" s="12"/>
+      <c r="I32" s="11" t="s">
+        <v>57</v>
+      </c>
+      <c r="J32" s="13"/>
     </row>
     <row r="33" spans="2:10" ht="15.6">
       <c r="B33" s="2" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="C33" s="5"/>
       <c r="D33" s="5"/>
-      <c r="E33" s="6" t="s">
-        <v>52</v>
-      </c>
+      <c r="E33" s="5"/>
       <c r="F33" s="5"/>
-      <c r="G33" s="5"/>
-      <c r="H33" s="11" t="s">
-        <v>56</v>
-      </c>
-      <c r="I33" s="12"/>
-      <c r="J33" s="13" t="s">
-        <v>100</v>
-      </c>
+      <c r="G33" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="H33" s="12"/>
+      <c r="I33" s="11" t="s">
+        <v>57</v>
+      </c>
+      <c r="J33" s="13"/>
     </row>
     <row r="34" spans="2:10" ht="15.6">
       <c r="B34" s="2" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="C34" s="5"/>
       <c r="D34" s="5"/>
-      <c r="E34" s="6" t="s">
-        <v>52</v>
-      </c>
+      <c r="E34" s="5"/>
       <c r="F34" s="5"/>
-      <c r="G34" s="5"/>
-      <c r="H34" s="11" t="s">
-        <v>56</v>
-      </c>
-      <c r="I34" s="12"/>
+      <c r="G34" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="H34" s="12"/>
+      <c r="I34" s="11" t="s">
+        <v>57</v>
+      </c>
       <c r="J34" s="13"/>
     </row>
-    <row r="35" spans="2:10" ht="15.6">
-      <c r="B35" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="C35" s="5"/>
-      <c r="D35" s="5"/>
-      <c r="E35" s="6" t="s">
-        <v>52</v>
-      </c>
-      <c r="F35" s="6" t="s">
-        <v>50</v>
-      </c>
-      <c r="G35" s="5"/>
-      <c r="H35" s="12"/>
-      <c r="I35" s="12"/>
+    <row r="35" spans="2:10" s="15" customFormat="1" ht="15.6">
+      <c r="B35" s="13"/>
+      <c r="C35" s="14"/>
+      <c r="D35" s="14"/>
+      <c r="E35" s="14"/>
+      <c r="F35" s="14"/>
+      <c r="G35" s="14"/>
+      <c r="H35" s="13"/>
+      <c r="I35" s="13"/>
       <c r="J35" s="13"/>
     </row>
     <row r="36" spans="2:10" ht="15.6">
       <c r="B36" s="2" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
       <c r="C36" s="5"/>
       <c r="D36" s="5"/>
       <c r="E36" s="6" t="s">
         <v>52</v>
       </c>
-      <c r="F36" s="6" t="s">
-        <v>50</v>
-      </c>
+      <c r="F36" s="5"/>
       <c r="G36" s="5"/>
-      <c r="H36" s="12"/>
+      <c r="H36" s="11" t="s">
+        <v>56</v>
+      </c>
       <c r="I36" s="12"/>
-      <c r="J36" s="13"/>
+      <c r="J36" s="13" t="s">
+        <v>100</v>
+      </c>
     </row>
     <row r="37" spans="2:10" ht="15.6">
       <c r="B37" s="2" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
       <c r="C37" s="5"/>
       <c r="D37" s="5"/>
       <c r="E37" s="6" t="s">
         <v>52</v>
       </c>
-      <c r="F37" s="6" t="s">
-        <v>50</v>
-      </c>
+      <c r="F37" s="5"/>
       <c r="G37" s="5"/>
-      <c r="H37" s="12"/>
+      <c r="H37" s="11" t="s">
+        <v>56</v>
+      </c>
       <c r="I37" s="12"/>
-      <c r="J37" s="13"/>
+      <c r="J37" s="13" t="s">
+        <v>100</v>
+      </c>
     </row>
     <row r="38" spans="2:10" ht="15.6">
       <c r="B38" s="2" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
       <c r="C38" s="5"/>
       <c r="D38" s="5"/>
       <c r="E38" s="6" t="s">
         <v>52</v>
       </c>
-      <c r="F38" s="6" t="s">
-        <v>50</v>
-      </c>
+      <c r="F38" s="5"/>
       <c r="G38" s="5"/>
-      <c r="H38" s="12"/>
+      <c r="H38" s="11" t="s">
+        <v>56</v>
+      </c>
       <c r="I38" s="12"/>
-      <c r="J38" s="13"/>
+      <c r="J38" s="13" t="s">
+        <v>100</v>
+      </c>
     </row>
     <row r="39" spans="2:10" ht="15.6">
       <c r="B39" s="2" t="s">
-        <v>36</v>
+        <v>30</v>
       </c>
       <c r="C39" s="5"/>
       <c r="D39" s="5"/>
-      <c r="E39" s="5"/>
+      <c r="E39" s="6" t="s">
+        <v>52</v>
+      </c>
       <c r="F39" s="5"/>
-      <c r="G39" s="6" t="s">
-        <v>49</v>
-      </c>
-      <c r="H39" s="12"/>
+      <c r="G39" s="5"/>
+      <c r="H39" s="11" t="s">
+        <v>56</v>
+      </c>
       <c r="I39" s="12"/>
-      <c r="J39" s="13"/>
+      <c r="J39" s="13" t="s">
+        <v>100</v>
+      </c>
     </row>
     <row r="40" spans="2:10" ht="15.6">
       <c r="B40" s="2" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="C40" s="5"/>
       <c r="D40" s="5"/>
-      <c r="E40" s="5"/>
+      <c r="E40" s="6" t="s">
+        <v>52</v>
+      </c>
       <c r="F40" s="5"/>
       <c r="G40" s="5"/>
-      <c r="H40" s="12"/>
+      <c r="H40" s="11" t="s">
+        <v>56</v>
+      </c>
       <c r="I40" s="12"/>
       <c r="J40" s="13"/>
     </row>
-    <row r="41" spans="2:10" ht="15.6">
-      <c r="B41" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="C41" s="5"/>
-      <c r="D41" s="5"/>
-      <c r="E41" s="5"/>
-      <c r="F41" s="5"/>
-      <c r="G41" s="6" t="s">
-        <v>49</v>
-      </c>
-      <c r="H41" s="12"/>
-      <c r="I41" s="12"/>
+    <row r="41" spans="2:10" s="15" customFormat="1" ht="15.6">
+      <c r="B41" s="13"/>
+      <c r="C41" s="14"/>
+      <c r="D41" s="14"/>
+      <c r="E41" s="14"/>
+      <c r="F41" s="14"/>
+      <c r="G41" s="14"/>
+      <c r="H41" s="13"/>
+      <c r="I41" s="13"/>
       <c r="J41" s="13"/>
     </row>
     <row r="42" spans="2:10" ht="15.6">
       <c r="B42" s="2" t="s">
-        <v>39</v>
+        <v>32</v>
       </c>
       <c r="C42" s="5"/>
       <c r="D42" s="5"/>
       <c r="E42" s="6" t="s">
         <v>52</v>
       </c>
-      <c r="F42" s="5"/>
+      <c r="F42" s="6" t="s">
+        <v>50</v>
+      </c>
       <c r="G42" s="5"/>
-      <c r="H42" s="11" t="s">
-        <v>56</v>
-      </c>
+      <c r="H42" s="12"/>
       <c r="I42" s="12"/>
       <c r="J42" s="13"/>
     </row>
     <row r="43" spans="2:10" ht="15.6">
       <c r="B43" s="2" t="s">
-        <v>40</v>
+        <v>33</v>
       </c>
       <c r="C43" s="5"/>
       <c r="D43" s="5"/>
       <c r="E43" s="6" t="s">
         <v>52</v>
       </c>
-      <c r="F43" s="5"/>
+      <c r="F43" s="6" t="s">
+        <v>50</v>
+      </c>
       <c r="G43" s="5"/>
-      <c r="H43" s="11" t="s">
-        <v>56</v>
-      </c>
+      <c r="H43" s="12"/>
       <c r="I43" s="12"/>
-      <c r="J43" s="13" t="s">
-        <v>100</v>
-      </c>
+      <c r="J43" s="13"/>
     </row>
     <row r="44" spans="2:10" ht="15.6">
       <c r="B44" s="2" t="s">
-        <v>41</v>
+        <v>34</v>
       </c>
       <c r="C44" s="5"/>
       <c r="D44" s="5"/>
-      <c r="E44" s="5"/>
-      <c r="F44" s="5"/>
+      <c r="E44" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="F44" s="6" t="s">
+        <v>50</v>
+      </c>
       <c r="G44" s="5"/>
-      <c r="H44" s="11" t="s">
-        <v>56</v>
-      </c>
+      <c r="H44" s="12"/>
       <c r="I44" s="12"/>
-      <c r="J44" s="13" t="s">
-        <v>100</v>
-      </c>
+      <c r="J44" s="13"/>
     </row>
     <row r="45" spans="2:10" ht="15.6">
       <c r="B45" s="2" t="s">
-        <v>42</v>
+        <v>35</v>
       </c>
       <c r="C45" s="5"/>
       <c r="D45" s="5"/>
       <c r="E45" s="6" t="s">
         <v>52</v>
       </c>
-      <c r="F45" s="5"/>
+      <c r="F45" s="6" t="s">
+        <v>50</v>
+      </c>
       <c r="G45" s="5"/>
-      <c r="H45" s="11" t="s">
-        <v>56</v>
-      </c>
+      <c r="H45" s="12"/>
       <c r="I45" s="12"/>
-      <c r="J45" s="13" t="s">
-        <v>100</v>
-      </c>
+      <c r="J45" s="13"/>
     </row>
     <row r="46" spans="2:10" ht="15.6">
       <c r="B46" s="2" t="s">
-        <v>43</v>
+        <v>36</v>
       </c>
       <c r="C46" s="5"/>
       <c r="D46" s="5"/>
-      <c r="E46" s="6" t="s">
-        <v>52</v>
-      </c>
+      <c r="E46" s="5"/>
       <c r="F46" s="5"/>
-      <c r="G46" s="5"/>
-      <c r="H46" s="11" t="s">
+      <c r="G46" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="H46" s="12"/>
+      <c r="I46" s="12"/>
+      <c r="J46" s="13"/>
+    </row>
+    <row r="47" spans="2:10" ht="15.6">
+      <c r="B47" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="C47" s="5"/>
+      <c r="D47" s="5"/>
+      <c r="E47" s="5"/>
+      <c r="F47" s="5"/>
+      <c r="G47" s="5"/>
+      <c r="H47" s="12"/>
+      <c r="I47" s="12"/>
+      <c r="J47" s="13"/>
+    </row>
+    <row r="48" spans="2:10" ht="15.6">
+      <c r="B48" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="C48" s="5"/>
+      <c r="D48" s="5"/>
+      <c r="E48" s="5"/>
+      <c r="F48" s="5"/>
+      <c r="G48" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="H48" s="12"/>
+      <c r="I48" s="12"/>
+      <c r="J48" s="13"/>
+    </row>
+    <row r="49" spans="2:10" ht="15.6">
+      <c r="B49" s="2"/>
+      <c r="C49" s="5"/>
+      <c r="D49" s="5"/>
+      <c r="E49" s="5"/>
+      <c r="F49" s="5"/>
+      <c r="G49" s="6"/>
+      <c r="H49" s="12"/>
+      <c r="I49" s="12"/>
+      <c r="J49" s="13"/>
+    </row>
+    <row r="50" spans="2:10" ht="15.6">
+      <c r="B50" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="C50" s="5"/>
+      <c r="D50" s="5"/>
+      <c r="E50" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="F50" s="5"/>
+      <c r="G50" s="5"/>
+      <c r="H50" s="11" t="s">
         <v>56</v>
       </c>
-      <c r="I46" s="12"/>
-      <c r="J46" s="13" t="s">
+      <c r="I50" s="12"/>
+      <c r="J50" s="13"/>
+    </row>
+    <row r="51" spans="2:10" ht="15.6">
+      <c r="B51" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="C51" s="5"/>
+      <c r="D51" s="5"/>
+      <c r="E51" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="F51" s="5"/>
+      <c r="G51" s="5"/>
+      <c r="H51" s="11" t="s">
+        <v>56</v>
+      </c>
+      <c r="I51" s="12"/>
+      <c r="J51" s="13" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="52" spans="2:10" ht="15.6">
+      <c r="B52" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="C52" s="5"/>
+      <c r="D52" s="5"/>
+      <c r="E52" s="5"/>
+      <c r="F52" s="5"/>
+      <c r="G52" s="5"/>
+      <c r="H52" s="11" t="s">
+        <v>56</v>
+      </c>
+      <c r="I52" s="12"/>
+      <c r="J52" s="13" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="53" spans="2:10" ht="15.6">
+      <c r="B53" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="C53" s="5"/>
+      <c r="D53" s="5"/>
+      <c r="E53" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="F53" s="5"/>
+      <c r="G53" s="5"/>
+      <c r="H53" s="11" t="s">
+        <v>56</v>
+      </c>
+      <c r="I53" s="12"/>
+      <c r="J53" s="13" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="54" spans="2:10" ht="15.6">
+      <c r="B54" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="C54" s="5"/>
+      <c r="D54" s="5"/>
+      <c r="E54" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="F54" s="5"/>
+      <c r="G54" s="5"/>
+      <c r="H54" s="11" t="s">
+        <v>56</v>
+      </c>
+      <c r="I54" s="12"/>
+      <c r="J54" s="13" t="s">
         <v>100</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Task List updated Role frontend changed.
</commit_message>
<xml_diff>
--- a/Role permissions.xlsx
+++ b/Role permissions.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21328"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5317565D-C43E-4E9E-8ECD-403EBE5314B7}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{43F7DB7A-0E91-49CC-B8E0-437E8F741218}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="240" uniqueCount="101">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="244" uniqueCount="101">
   <si>
     <t>/compound/add [GET]</t>
   </si>
@@ -804,8 +804,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B2:R54"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K21" sqref="K21"/>
+    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
+      <selection activeCell="G42" sqref="G42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -1398,7 +1398,9 @@
       <c r="G22" s="6" t="s">
         <v>49</v>
       </c>
-      <c r="H22" s="12"/>
+      <c r="H22" s="11" t="s">
+        <v>56</v>
+      </c>
       <c r="I22" s="12"/>
       <c r="J22" s="13" t="s">
         <v>100</v>
@@ -1438,7 +1440,9 @@
       <c r="G23" s="6" t="s">
         <v>49</v>
       </c>
-      <c r="H23" s="12"/>
+      <c r="H23" s="11" t="s">
+        <v>56</v>
+      </c>
       <c r="I23" s="12"/>
       <c r="J23" s="13" t="s">
         <v>100</v>
@@ -1478,7 +1482,9 @@
       <c r="G24" s="6" t="s">
         <v>49</v>
       </c>
-      <c r="H24" s="12"/>
+      <c r="H24" s="11" t="s">
+        <v>56</v>
+      </c>
       <c r="I24" s="12"/>
       <c r="J24" s="13" t="s">
         <v>100</v>
@@ -1764,7 +1770,9 @@
         <v>56</v>
       </c>
       <c r="I40" s="12"/>
-      <c r="J40" s="13"/>
+      <c r="J40" s="13" t="s">
+        <v>100</v>
+      </c>
     </row>
     <row r="41" spans="2:10" s="15" customFormat="1" ht="15.6">
       <c r="B41" s="13"/>

</xml_diff>